<commit_message>
fix: skripsi bab 4
</commit_message>
<xml_diff>
--- a/DOKUMENT/kelayakan.xlsx
+++ b/DOKUMENT/kelayakan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SKRIPSI\DOKUMENT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51902EC3-0DC8-4D1C-9206-A96196BFC52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1017C69-1207-427C-8711-55C24CFB823A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="220">
   <si>
     <t>Timestamp</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Apakah website ini sangat mudah untuk dipelajari?</t>
-  </si>
-  <si>
-    <t>Apakah Anda merasa mudah untuk belajar menggunakan website ini?</t>
   </si>
   <si>
     <t>Apakah setelah menggunakan website ini, Anda merasa lebih familiar dengan tata cara penggunaannya?</t>
@@ -687,14 +684,24 @@
   </si>
   <si>
     <t>Uji validitas</t>
+  </si>
+  <si>
+    <t>total varian</t>
+  </si>
+  <si>
+    <t>varian total</t>
+  </si>
+  <si>
+    <t>Apakah hasil deteksi yang dilakukan sesuai dengan objek yang dideteksi?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="173" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -868,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -892,33 +899,39 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,11 +1152,11 @@
   </sheetPr>
   <dimension ref="A1:R92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomRight" activeCell="N62" sqref="N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1194,22 +1207,22 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="204.75" x14ac:dyDescent="0.25">
@@ -1217,11 +1230,11 @@
         <v>45406.60993741898</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="1">
         <v>4</v>
       </c>
@@ -1250,23 +1263,23 @@
         <v>4</v>
       </c>
       <c r="M2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" s="1">
         <v>4</v>
       </c>
       <c r="O2" s="2">
         <f>SUM(D2:N2)</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
@@ -1274,10 +1287,10 @@
         <v>45406.610808055557</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D3" s="1">
         <v>4</v>
@@ -1317,13 +1330,13 @@
         <v>43</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="173.25" x14ac:dyDescent="0.25">
@@ -1331,10 +1344,10 @@
         <v>45406.610994456016</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1">
         <v>4</v>
@@ -1364,23 +1377,23 @@
         <v>4</v>
       </c>
       <c r="M4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N4" s="1">
         <v>4</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1388,10 +1401,10 @@
         <v>45406.615400509254</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
@@ -1431,11 +1444,11 @@
         <v>42</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1443,10 +1456,10 @@
         <v>45406.617954108791</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1">
         <v>4</v>
@@ -1488,7 +1501,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1496,10 +1509,10 @@
         <v>45406.620574513887</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -1539,13 +1552,13 @@
         <v>41</v>
       </c>
       <c r="P7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
@@ -1553,10 +1566,10 @@
         <v>45406.622312939813</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1">
         <v>4</v>
@@ -1586,23 +1599,23 @@
         <v>4</v>
       </c>
       <c r="M8" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N8" s="1">
         <v>4</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1610,10 +1623,10 @@
         <v>45406.624082083334</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
@@ -1661,10 +1674,10 @@
         <v>45406.626823877319</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
@@ -1704,10 +1717,10 @@
         <v>42</v>
       </c>
       <c r="P10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="R10" s="1"/>
     </row>
@@ -1716,10 +1729,10 @@
         <v>45406.648065972222</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1">
         <v>4</v>
@@ -1759,13 +1772,13 @@
         <v>43</v>
       </c>
       <c r="P11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
@@ -1773,10 +1786,10 @@
         <v>45406.650304328708</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
@@ -1806,23 +1819,23 @@
         <v>4</v>
       </c>
       <c r="M12" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" s="1">
         <v>4</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="47.25" x14ac:dyDescent="0.25">
@@ -1830,10 +1843,10 @@
         <v>45406.658231990739</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
@@ -1873,13 +1886,13 @@
         <v>40</v>
       </c>
       <c r="P13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="173.25" x14ac:dyDescent="0.25">
@@ -1887,10 +1900,10 @@
         <v>45406.722871921302</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1">
         <v>4</v>
@@ -1930,13 +1943,13 @@
         <v>40</v>
       </c>
       <c r="P14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1944,10 +1957,10 @@
         <v>45406.731196180554</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1">
         <v>4</v>
@@ -1989,7 +2002,7 @@
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
@@ -1997,10 +2010,10 @@
         <v>45406.761491412035</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1">
         <v>3</v>
@@ -2040,13 +2053,13 @@
         <v>36</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="94.5" x14ac:dyDescent="0.25">
@@ -2054,10 +2067,10 @@
         <v>45406.765710763888</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1">
         <v>4</v>
@@ -2097,13 +2110,13 @@
         <v>44</v>
       </c>
       <c r="P17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2111,10 +2124,10 @@
         <v>45406.767121990742</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1">
         <v>4</v>
@@ -2154,13 +2167,13 @@
         <v>40</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="78.75" x14ac:dyDescent="0.25">
@@ -2168,10 +2181,10 @@
         <v>45406.768109340279</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1">
         <v>3</v>
@@ -2201,23 +2214,23 @@
         <v>3</v>
       </c>
       <c r="M19" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N19" s="1">
         <v>4</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R19" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
@@ -2225,10 +2238,10 @@
         <v>45406.772431006946</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
@@ -2258,30 +2271,30 @@
         <v>4</v>
       </c>
       <c r="M20" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N20" s="1">
         <v>4</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>45406.7740753588</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
@@ -2321,13 +2334,13 @@
         <v>41</v>
       </c>
       <c r="P21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
@@ -2335,10 +2348,10 @@
         <v>45406.776267638888</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
@@ -2378,13 +2391,13 @@
         <v>39</v>
       </c>
       <c r="P22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="94.5" x14ac:dyDescent="0.25">
@@ -2392,10 +2405,10 @@
         <v>45406.814137453708</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
@@ -2425,23 +2438,23 @@
         <v>4</v>
       </c>
       <c r="M23" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N23" s="1">
         <v>4</v>
       </c>
       <c r="O23" s="2">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="157.5" x14ac:dyDescent="0.25">
@@ -2449,10 +2462,10 @@
         <v>45406.870665104172</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="1">
         <v>4</v>
@@ -2492,13 +2505,13 @@
         <v>43</v>
       </c>
       <c r="P24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2506,10 +2519,10 @@
         <v>45406.871017210651</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1">
         <v>3</v>
@@ -2549,7 +2562,7 @@
         <v>34</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
@@ -2559,10 +2572,10 @@
         <v>45406.893882488424</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="1">
         <v>3</v>
@@ -2602,13 +2615,13 @@
         <v>33</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="R26" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="299.25" x14ac:dyDescent="0.25">
@@ -2616,10 +2629,10 @@
         <v>45406.992285405096</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" s="1">
         <v>4</v>
@@ -2659,13 +2672,13 @@
         <v>43</v>
       </c>
       <c r="P27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q27" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="R27" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2673,10 +2686,10 @@
         <v>45407.477807974537</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1">
         <v>4</v>
@@ -2716,24 +2729,24 @@
         <v>37</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>45407.585353391201</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="1">
         <v>4</v>
@@ -2773,24 +2786,24 @@
         <v>44</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="126" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>45407.708176087966</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" s="1">
         <v>4</v>
@@ -2830,24 +2843,24 @@
         <v>41</v>
       </c>
       <c r="P30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q30" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="R30" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:18" ht="126" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>45407.711063935189</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31" s="1">
         <v>4</v>
@@ -2887,13 +2900,13 @@
         <v>41</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q31" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="R31" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="110.25" x14ac:dyDescent="0.25">
@@ -2901,10 +2914,10 @@
         <v>45407.809315439816</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32" s="1">
         <v>3</v>
@@ -2944,13 +2957,13 @@
         <v>41</v>
       </c>
       <c r="P32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q32" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="R32" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2958,10 +2971,10 @@
         <v>45407.969695011576</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D33" s="5">
         <v>4</v>
@@ -3001,13 +3014,13 @@
         <v>39</v>
       </c>
       <c r="P33" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q33" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="R33" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="R33" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -3015,10 +3028,10 @@
         <v>45408.634623194448</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" s="5">
         <v>4</v>
@@ -3058,13 +3071,13 @@
         <v>43</v>
       </c>
       <c r="P34" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q34" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="R34" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="R34" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -3072,10 +3085,10 @@
         <v>45410.968659837963</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D35" s="5">
         <v>4</v>
@@ -3105,23 +3118,23 @@
         <v>4</v>
       </c>
       <c r="M35" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N35" s="5">
         <v>4</v>
       </c>
       <c r="O35" s="2">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P35" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q35" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R35" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -3129,10 +3142,10 @@
         <v>45412.498534988423</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36" s="5">
         <v>4</v>
@@ -3172,7 +3185,7 @@
         <v>39</v>
       </c>
       <c r="R36" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -3180,10 +3193,10 @@
         <v>45412.637872465275</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" s="5">
         <v>4</v>
@@ -3223,13 +3236,13 @@
         <v>44</v>
       </c>
       <c r="P37" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q37" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="R37" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="R37" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -3237,10 +3250,10 @@
         <v>45412.665930162038</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="D38" s="5">
         <v>4</v>
@@ -3282,64 +3295,64 @@
     </row>
     <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="D41" s="7">
         <f>CORREL(D2:D38,$O$2:$O$38)</f>
-        <v>0.71601193022079856</v>
+        <v>0.72563739729491694</v>
       </c>
       <c r="E41" s="7">
         <f t="shared" ref="E41:N41" si="1">CORREL(E2:E38,$O$2:$O$38)</f>
-        <v>0.63837864127591259</v>
+        <v>0.64106806895059265</v>
       </c>
       <c r="F41" s="7">
         <f t="shared" si="1"/>
-        <v>0.67246216373791567</v>
+        <v>0.64997963769010836</v>
       </c>
       <c r="G41" s="7">
         <f t="shared" si="1"/>
-        <v>0.48409219629928402</v>
+        <v>0.48728210542495792</v>
       </c>
       <c r="H41" s="7">
         <f t="shared" si="1"/>
-        <v>0.48381679967119645</v>
+        <v>0.47271390776045524</v>
       </c>
       <c r="I41" s="7">
         <f t="shared" si="1"/>
-        <v>0.54976718141424885</v>
+        <v>0.55840910477114936</v>
       </c>
       <c r="J41" s="7">
         <f t="shared" si="1"/>
-        <v>0.55028727987906934</v>
+        <v>0.58381532708079398</v>
       </c>
       <c r="K41" s="7">
         <f t="shared" si="1"/>
-        <v>0.40165156008758279</v>
+        <v>0.3791991782780163</v>
       </c>
       <c r="L41" s="7">
         <f t="shared" si="1"/>
-        <v>0.71481739501805408</v>
+        <v>0.70921950691768376</v>
       </c>
       <c r="M41" s="7">
         <f t="shared" si="1"/>
-        <v>0.61993635263962033</v>
+        <v>0.48722352937078695</v>
       </c>
       <c r="N41" s="7">
         <f t="shared" si="1"/>
-        <v>0.63837864127591271</v>
-      </c>
-      <c r="O41" s="29"/>
-      <c r="P41" s="29"/>
+        <v>0.61420564703533564</v>
+      </c>
+      <c r="O41" s="28"/>
+      <c r="P41" s="28"/>
     </row>
     <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D42" s="7">
         <v>0.41799999999999998</v>
@@ -3374,13 +3387,13 @@
       <c r="N42" s="7">
         <v>0.32500000000000001</v>
       </c>
-      <c r="O42" s="29"/>
-      <c r="P42" s="29"/>
+      <c r="O42" s="28"/>
+      <c r="P42" s="28"/>
     </row>
     <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D43" s="7" t="str">
         <f>IF(D41&gt;D42,"VALID","TIDAK VALID")</f>
@@ -3426,18 +3439,18 @@
         <f t="shared" si="2"/>
         <v>VALID</v>
       </c>
-      <c r="O43" s="30">
+      <c r="O43" s="29">
         <f>VAR(O2:O38)</f>
-        <v>7.9159159159159156</v>
-      </c>
-      <c r="P43" s="30" t="s">
-        <v>134</v>
+        <v>7.6576576576576558</v>
+      </c>
+      <c r="P43" s="29" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
       <c r="C44" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D44" s="7">
         <f>VAR(D2:D38)</f>
@@ -3477,28 +3490,28 @@
       </c>
       <c r="M44" s="7">
         <f t="shared" si="3"/>
-        <v>0.20270270270270252</v>
+        <v>0.25675675675675635</v>
       </c>
       <c r="N44" s="7">
         <f t="shared" si="3"/>
         <v>0.1396396396396396</v>
       </c>
-      <c r="O44" s="30">
+      <c r="O44" s="29">
         <f>SUM(D44:N44)</f>
-        <v>2.1771771771771804</v>
-      </c>
-      <c r="P44" s="30" t="s">
-        <v>135</v>
+        <v>2.2312312312312343</v>
+      </c>
+      <c r="P44" s="29" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46" s="9"/>
+        <v>135</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" s="33"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="11"/>
@@ -3506,31 +3519,31 @@
     <row r="47" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="12"/>
       <c r="C47" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="E47" s="13"/>
       <c r="F47" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="12"/>
       <c r="C48" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>140</v>
       </c>
       <c r="E48" s="13"/>
       <c r="F48" s="13">
         <f>11/10*(1-O44/O43)</f>
-        <v>0.79745827010622117</v>
+        <v>0.77949019607843095</v>
       </c>
       <c r="G48" s="14" t="str">
         <f>IF(AND(F48&gt;0.8,F48&lt;=1), "Reliabilias Sangat Tinggi", IF(AND(F48&gt;0.6,F48&lt;=0.8),"Relibilitas Tinggi",IF(AND(F48&gt;0.4,F48&lt;=0.6),"Relibilitas Sedang",IF(AND(F48&gt;0.2,F48&lt;=0.4),"Relibilitas Rendah",IF(AND(F48&gt;0,F48&lt;=0.2),"Tidak Reliabel","")))))</f>
@@ -3540,10 +3553,10 @@
     <row r="49" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="12"/>
       <c r="C49" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>142</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -3552,10 +3565,10 @@
     <row r="50" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="12"/>
       <c r="C50" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -3564,10 +3577,10 @@
     <row r="51" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="12"/>
       <c r="C51" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="D51" s="13" t="s">
-        <v>146</v>
       </c>
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
@@ -3583,800 +3596,800 @@
     </row>
     <row r="54" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D54" s="34"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="I54" s="20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="21"/>
+      <c r="C55" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="C54" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D54" s="19"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G54" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="H54" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="I54" s="21" t="s">
+      <c r="D55" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="55" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="22"/>
-      <c r="C55" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="D55" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="G55" s="24">
+      <c r="G55" s="23">
         <v>44</v>
       </c>
-      <c r="H55" s="24">
+      <c r="H55" s="23">
         <f>(O2/G55)*100</f>
-        <v>95.454545454545453</v>
-      </c>
-      <c r="I55" s="25" t="str">
+        <v>93.181818181818173</v>
+      </c>
+      <c r="I55" s="24" t="str">
         <f>IF(AND(H55&gt;0,H55&lt;=20),"SANGAT TIDAK LAYAK",IF(AND(H55&gt;20,H55&lt;=40),"TIDAK LAYAK",IF(AND(H55&gt;40,H55&lt;=60),"CUKUP",IF(AND(H55&gt;60,H55&lt;=80),"LAYAK",IF(AND(H55&gt;80,H55&lt;=100),"SANGAT LAYAK","")))))</f>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
     <row r="56" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="22"/>
-      <c r="C56" s="23" t="s">
+      <c r="B56" s="21"/>
+      <c r="C56" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="D56" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="G56" s="24">
+      <c r="E56" s="23"/>
+      <c r="F56" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G56" s="23">
         <v>44</v>
       </c>
-      <c r="H56" s="24">
+      <c r="H56" s="23">
         <f t="shared" ref="H56:H91" si="4">(O3/G56)*100</f>
         <v>97.727272727272734</v>
       </c>
-      <c r="I56" s="25" t="str">
+      <c r="I56" s="24" t="str">
         <f t="shared" ref="I56:I92" si="5">IF(AND(H56&gt;0,H56&lt;=20),"SANGAT TIDAK LAYAK",IF(AND(H56&gt;20,H56&lt;=40),"TIDAK LAYAK",IF(AND(H56&gt;40,H56&lt;=60),"CUKUP",IF(AND(H56&gt;60,H56&lt;=80),"LAYAK",IF(AND(H56&gt;80,H56&lt;=100),"SANGAT LAYAK","")))))</f>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
     <row r="57" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="22"/>
-      <c r="C57" s="23" t="s">
+      <c r="B57" s="21"/>
+      <c r="C57" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="D57" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="E57" s="23"/>
+      <c r="F57" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G57" s="23">
+        <v>44</v>
+      </c>
+      <c r="H57" s="23">
+        <f t="shared" si="4"/>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I57" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="21"/>
+      <c r="C58" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24" t="s">
+      <c r="D58" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="G57" s="24">
+      <c r="G58" s="23">
         <v>44</v>
       </c>
-      <c r="H57" s="24">
+      <c r="H58" s="23">
+        <f t="shared" si="4"/>
+        <v>95.454545454545453</v>
+      </c>
+      <c r="I58" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="21"/>
+      <c r="C59" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59" s="23">
+        <v>44</v>
+      </c>
+      <c r="H59" s="23">
+        <f t="shared" si="4"/>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I59" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="21"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="G60" s="23">
+        <v>44</v>
+      </c>
+      <c r="H60" s="23">
+        <f t="shared" si="4"/>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="I60" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="21"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="G61" s="23">
+        <v>44</v>
+      </c>
+      <c r="H61" s="23">
+        <f t="shared" si="4"/>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I61" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="21"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="G62" s="23">
+        <v>44</v>
+      </c>
+      <c r="H62" s="23">
+        <f t="shared" si="4"/>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="I62" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="21"/>
+      <c r="C63" s="23"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G63" s="23">
+        <v>44</v>
+      </c>
+      <c r="H63" s="23">
+        <f t="shared" si="4"/>
+        <v>95.454545454545453</v>
+      </c>
+      <c r="I63" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="21"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="G64" s="23">
+        <v>44</v>
+      </c>
+      <c r="H64" s="23">
+        <f t="shared" si="4"/>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I64" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="21"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="G65" s="23">
+        <v>44</v>
+      </c>
+      <c r="H65" s="23">
+        <f t="shared" si="4"/>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="I65" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="21"/>
+      <c r="C66" s="23"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="G66" s="23">
+        <v>44</v>
+      </c>
+      <c r="H66" s="23">
+        <f t="shared" si="4"/>
+        <v>90.909090909090907</v>
+      </c>
+      <c r="I66" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="21"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G67" s="23">
+        <v>44</v>
+      </c>
+      <c r="H67" s="23">
+        <f t="shared" si="4"/>
+        <v>90.909090909090907</v>
+      </c>
+      <c r="I67" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="21"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="G68" s="23">
+        <v>44</v>
+      </c>
+      <c r="H68" s="23">
+        <f t="shared" si="4"/>
+        <v>95.454545454545453</v>
+      </c>
+      <c r="I68" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="21"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G69" s="23">
+        <v>44</v>
+      </c>
+      <c r="H69" s="23">
+        <f t="shared" si="4"/>
+        <v>81.818181818181827</v>
+      </c>
+      <c r="I69" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="21"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="G70" s="23">
+        <v>44</v>
+      </c>
+      <c r="H70" s="23">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="I57" s="25" t="str">
+      <c r="I70" s="24" t="str">
         <f t="shared" si="5"/>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="22"/>
-      <c r="C58" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="D58" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="G58" s="24">
+    <row r="71" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="21"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G71" s="23">
         <v>44</v>
       </c>
-      <c r="H58" s="24">
+      <c r="H71" s="23">
+        <f t="shared" si="4"/>
+        <v>90.909090909090907</v>
+      </c>
+      <c r="I71" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="21"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="G72" s="23">
+        <v>44</v>
+      </c>
+      <c r="H72" s="23">
+        <f t="shared" si="4"/>
+        <v>79.545454545454547</v>
+      </c>
+      <c r="I72" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="21"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="G73" s="23">
+        <v>44</v>
+      </c>
+      <c r="H73" s="23">
+        <f t="shared" si="4"/>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I73" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="21"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="G74" s="23">
+        <v>44</v>
+      </c>
+      <c r="H74" s="23">
+        <f t="shared" si="4"/>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="I74" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="21"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="G75" s="23">
+        <v>44</v>
+      </c>
+      <c r="H75" s="23">
+        <f t="shared" si="4"/>
+        <v>88.63636363636364</v>
+      </c>
+      <c r="I75" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="21"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="G76" s="23">
+        <v>44</v>
+      </c>
+      <c r="H76" s="23">
         <f t="shared" si="4"/>
         <v>95.454545454545453</v>
       </c>
-      <c r="I58" s="25" t="str">
+      <c r="I76" s="24" t="str">
         <f t="shared" si="5"/>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
-    <row r="59" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="22"/>
-      <c r="C59" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="D59" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="G59" s="24">
+    <row r="77" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="21"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="G77" s="23">
         <v>44</v>
       </c>
-      <c r="H59" s="24">
+      <c r="H77" s="23">
         <f t="shared" si="4"/>
         <v>97.727272727272734</v>
       </c>
-      <c r="I59" s="25" t="str">
+      <c r="I77" s="24" t="str">
         <f t="shared" si="5"/>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
-    <row r="60" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="22"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="G60" s="24">
+    <row r="78" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="21"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G78" s="23">
         <v>44</v>
       </c>
-      <c r="H60" s="24">
+      <c r="H78" s="23">
+        <f t="shared" si="4"/>
+        <v>77.272727272727266</v>
+      </c>
+      <c r="I78" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="21"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G79" s="23">
+        <v>44</v>
+      </c>
+      <c r="H79" s="23">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="I79" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>LAYAK</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="21"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="G80" s="23">
+        <v>44</v>
+      </c>
+      <c r="H80" s="23">
+        <f t="shared" si="4"/>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I80" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="21"/>
+      <c r="C81" s="23"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="G81" s="23">
+        <v>44</v>
+      </c>
+      <c r="H81" s="23">
+        <f t="shared" si="4"/>
+        <v>84.090909090909093</v>
+      </c>
+      <c r="I81" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="21"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="G82" s="23">
+        <v>44</v>
+      </c>
+      <c r="H82" s="23">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="I82" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="21"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23" t="s">
+        <v>192</v>
+      </c>
+      <c r="G83" s="23">
+        <v>44</v>
+      </c>
+      <c r="H83" s="23">
         <f t="shared" si="4"/>
         <v>93.181818181818173</v>
       </c>
-      <c r="I60" s="25" t="str">
+      <c r="I83" s="24" t="str">
         <f t="shared" si="5"/>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="22"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="G61" s="24">
+    <row r="84" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="21"/>
+      <c r="C84" s="23"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="G84" s="23">
         <v>44</v>
       </c>
-      <c r="H61" s="24">
+      <c r="H84" s="23">
+        <f t="shared" si="4"/>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="I84" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="21"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G85" s="23">
+        <v>44</v>
+      </c>
+      <c r="H85" s="23">
+        <f t="shared" si="4"/>
+        <v>93.181818181818173</v>
+      </c>
+      <c r="I85" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="21"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="G86" s="23">
+        <v>44</v>
+      </c>
+      <c r="H86" s="23">
+        <f t="shared" si="4"/>
+        <v>88.63636363636364</v>
+      </c>
+      <c r="I86" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="21"/>
+      <c r="C87" s="23"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="G87" s="23">
+        <v>44</v>
+      </c>
+      <c r="H87" s="23">
+        <f t="shared" si="4"/>
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I87" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="21"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="G88" s="23">
+        <v>44</v>
+      </c>
+      <c r="H88" s="23">
+        <f t="shared" si="4"/>
+        <v>90.909090909090907</v>
+      </c>
+      <c r="I88" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="21"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="G89" s="23">
+        <v>44</v>
+      </c>
+      <c r="H89" s="23">
+        <f t="shared" si="4"/>
+        <v>88.63636363636364</v>
+      </c>
+      <c r="I89" s="24" t="str">
+        <f t="shared" si="5"/>
+        <v>SANGAT LAYAK</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="21"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="G90" s="23">
+        <v>44</v>
+      </c>
+      <c r="H90" s="23">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="I61" s="25" t="str">
+      <c r="I90" s="24" t="str">
         <f t="shared" si="5"/>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="22"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="G62" s="24">
+    <row r="91" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="21"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="G91" s="23">
         <v>44</v>
       </c>
-      <c r="H62" s="24">
+      <c r="H91" s="23">
         <f t="shared" si="4"/>
-        <v>93.181818181818173</v>
-      </c>
-      <c r="I62" s="25" t="str">
+        <v>97.727272727272734</v>
+      </c>
+      <c r="I91" s="24" t="str">
         <f t="shared" si="5"/>
         <v>SANGAT LAYAK</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="22"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="G63" s="24">
-        <v>44</v>
-      </c>
-      <c r="H63" s="24">
-        <f t="shared" si="4"/>
-        <v>95.454545454545453</v>
-      </c>
-      <c r="I63" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="22"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="G64" s="24">
-        <v>44</v>
-      </c>
-      <c r="H64" s="24">
-        <f t="shared" si="4"/>
-        <v>97.727272727272734</v>
-      </c>
-      <c r="I64" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="22"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="G65" s="24">
-        <v>44</v>
-      </c>
-      <c r="H65" s="24">
-        <f t="shared" si="4"/>
-        <v>95.454545454545453</v>
-      </c>
-      <c r="I65" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="22"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="G66" s="24">
-        <v>44</v>
-      </c>
-      <c r="H66" s="24">
-        <f t="shared" si="4"/>
-        <v>90.909090909090907</v>
-      </c>
-      <c r="I66" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="22"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="G67" s="24">
-        <v>44</v>
-      </c>
-      <c r="H67" s="24">
-        <f t="shared" si="4"/>
-        <v>90.909090909090907</v>
-      </c>
-      <c r="I67" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="22"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="G68" s="24">
-        <v>44</v>
-      </c>
-      <c r="H68" s="24">
-        <f t="shared" si="4"/>
-        <v>95.454545454545453</v>
-      </c>
-      <c r="I68" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="22"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="G69" s="24">
-        <v>44</v>
-      </c>
-      <c r="H69" s="24">
-        <f t="shared" si="4"/>
-        <v>81.818181818181827</v>
-      </c>
-      <c r="I69" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="70" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="22"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="G70" s="24">
-        <v>44</v>
-      </c>
-      <c r="H70" s="24">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="I70" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="71" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="22"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="G71" s="24">
-        <v>44</v>
-      </c>
-      <c r="H71" s="24">
-        <f t="shared" si="4"/>
-        <v>90.909090909090907</v>
-      </c>
-      <c r="I71" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="22"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="G72" s="24">
-        <v>44</v>
-      </c>
-      <c r="H72" s="24">
-        <f t="shared" si="4"/>
-        <v>81.818181818181827</v>
-      </c>
-      <c r="I72" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="73" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="22"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="G73" s="24">
-        <v>44</v>
-      </c>
-      <c r="H73" s="24">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="I73" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="22"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="G74" s="24">
-        <v>44</v>
-      </c>
-      <c r="H74" s="24">
-        <f t="shared" si="4"/>
-        <v>93.181818181818173</v>
-      </c>
-      <c r="I74" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="22"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="G75" s="24">
-        <v>44</v>
-      </c>
-      <c r="H75" s="24">
-        <f t="shared" si="4"/>
-        <v>88.63636363636364</v>
-      </c>
-      <c r="I75" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="22"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="G76" s="24">
-        <v>44</v>
-      </c>
-      <c r="H76" s="24">
-        <f t="shared" si="4"/>
-        <v>97.727272727272734</v>
-      </c>
-      <c r="I76" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="22"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="G77" s="24">
-        <v>44</v>
-      </c>
-      <c r="H77" s="24">
-        <f t="shared" si="4"/>
-        <v>97.727272727272734</v>
-      </c>
-      <c r="I77" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="22"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="G78" s="24">
-        <v>44</v>
-      </c>
-      <c r="H78" s="24">
-        <f t="shared" si="4"/>
-        <v>77.272727272727266</v>
-      </c>
-      <c r="I78" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>LAYAK</v>
-      </c>
-    </row>
-    <row r="79" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="22"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="G79" s="24">
-        <v>44</v>
-      </c>
-      <c r="H79" s="24">
-        <f t="shared" si="4"/>
-        <v>75</v>
-      </c>
-      <c r="I79" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>LAYAK</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="22"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="G80" s="24">
-        <v>44</v>
-      </c>
-      <c r="H80" s="24">
-        <f t="shared" si="4"/>
-        <v>97.727272727272734</v>
-      </c>
-      <c r="I80" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="22"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="G81" s="24">
-        <v>44</v>
-      </c>
-      <c r="H81" s="24">
-        <f t="shared" si="4"/>
-        <v>84.090909090909093</v>
-      </c>
-      <c r="I81" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="22"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="G82" s="24">
-        <v>44</v>
-      </c>
-      <c r="H82" s="24">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="I82" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="22"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="G83" s="24">
-        <v>44</v>
-      </c>
-      <c r="H83" s="24">
-        <f t="shared" si="4"/>
-        <v>93.181818181818173</v>
-      </c>
-      <c r="I83" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="22"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="G84" s="24">
-        <v>44</v>
-      </c>
-      <c r="H84" s="24">
-        <f t="shared" si="4"/>
-        <v>93.181818181818173</v>
-      </c>
-      <c r="I84" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="85" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="22"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="G85" s="24">
-        <v>44</v>
-      </c>
-      <c r="H85" s="24">
-        <f t="shared" si="4"/>
-        <v>93.181818181818173</v>
-      </c>
-      <c r="I85" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="86" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="22"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="G86" s="24">
-        <v>44</v>
-      </c>
-      <c r="H86" s="24">
-        <f t="shared" si="4"/>
-        <v>88.63636363636364</v>
-      </c>
-      <c r="I86" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="87" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="22"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="G87" s="24">
-        <v>44</v>
-      </c>
-      <c r="H87" s="24">
-        <f t="shared" si="4"/>
-        <v>97.727272727272734</v>
-      </c>
-      <c r="I87" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="88" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="22"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="G88" s="24">
-        <v>44</v>
-      </c>
-      <c r="H88" s="24">
-        <f t="shared" si="4"/>
-        <v>93.181818181818173</v>
-      </c>
-      <c r="I88" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="89" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="22"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="G89" s="24">
-        <v>44</v>
-      </c>
-      <c r="H89" s="24">
-        <f t="shared" si="4"/>
-        <v>88.63636363636364</v>
-      </c>
-      <c r="I89" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="90" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="22"/>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="G90" s="24">
-        <v>44</v>
-      </c>
-      <c r="H90" s="24">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="I90" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="91" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="22"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24" t="s">
+    <row r="92" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="25"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
+      <c r="F92" s="26"/>
+      <c r="G92" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="G91" s="24">
-        <v>44</v>
-      </c>
-      <c r="H91" s="24">
-        <f t="shared" si="4"/>
-        <v>97.727272727272734</v>
-      </c>
-      <c r="I91" s="25" t="str">
-        <f t="shared" si="5"/>
-        <v>SANGAT LAYAK</v>
-      </c>
-    </row>
-    <row r="92" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="26"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="27" t="s">
-        <v>202</v>
-      </c>
-      <c r="H92" s="27">
+      <c r="H92" s="26">
         <f>AVERAGE(H55:H91)</f>
-        <v>93.243243243243199</v>
-      </c>
-      <c r="I92" s="28" t="str">
+        <v>92.751842751842716</v>
+      </c>
+      <c r="I92" s="27" t="str">
         <f t="shared" si="5"/>
         <v>SANGAT LAYAK</v>
       </c>
@@ -4394,69 +4407,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CEF6905-84EA-4998-A96D-B168CF5C9440}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="K1" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="L1" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="M1" s="31" t="s">
-        <v>216</v>
-      </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
-        <v>165</v>
+      <c r="A2" s="30" t="s">
+        <v>164</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
@@ -4486,61 +4493,61 @@
         <v>4</v>
       </c>
       <c r="K2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" s="1">
         <v>3</v>
       </c>
       <c r="M2">
         <f>SUM(B2:L2)</f>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M21" si="0">SUM(B3:L3)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
         <v>166</v>
-      </c>
-      <c r="B3" s="1">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1">
-        <v>3</v>
-      </c>
-      <c r="G3" s="1">
-        <v>3</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>3</v>
-      </c>
-      <c r="J3" s="1">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1">
-        <v>4</v>
-      </c>
-      <c r="L3" s="1">
-        <v>4</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M11" si="0">SUM(B3:L3)</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>167</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
@@ -4581,8 +4588,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
-        <v>168</v>
+      <c r="A5" s="30" t="s">
+        <v>167</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -4612,19 +4619,19 @@
         <v>4</v>
       </c>
       <c r="K5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L5" s="1">
         <v>4</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>169</v>
+      <c r="A6" s="30" t="s">
+        <v>168</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
@@ -4665,8 +4672,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>170</v>
+      <c r="A7" s="30" t="s">
+        <v>169</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -4707,8 +4714,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>171</v>
+      <c r="A8" s="30" t="s">
+        <v>170</v>
       </c>
       <c r="B8" s="1">
         <v>4</v>
@@ -4749,8 +4756,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
-        <v>172</v>
+      <c r="A9" s="30" t="s">
+        <v>171</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -4791,8 +4798,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>173</v>
+      <c r="A10" s="30" t="s">
+        <v>172</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
@@ -4833,8 +4840,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="31" t="s">
-        <v>174</v>
+      <c r="A11" s="30" t="s">
+        <v>173</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
@@ -4864,183 +4871,732 @@
         <v>4</v>
       </c>
       <c r="K11" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" s="1">
         <v>4</v>
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4</v>
+      </c>
+      <c r="I12" s="1">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1">
+        <v>4</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3</v>
+      </c>
+      <c r="L12" s="1">
+        <v>4</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3</v>
+      </c>
+      <c r="L14" s="1">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4</v>
+      </c>
+      <c r="K15" s="1">
+        <v>4</v>
+      </c>
+      <c r="L15" s="1">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="32" t="s">
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1">
+        <v>4</v>
+      </c>
+      <c r="K16" s="1">
+        <v>3</v>
+      </c>
+      <c r="L16" s="1">
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>4</v>
+      </c>
+      <c r="J18" s="1">
+        <v>3</v>
+      </c>
+      <c r="K18" s="1">
+        <v>3</v>
+      </c>
+      <c r="L18" s="1">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
+      <c r="H19" s="1">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1">
+        <v>3</v>
+      </c>
+      <c r="L19" s="1">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1">
+        <v>3</v>
+      </c>
+      <c r="G20" s="1">
+        <v>3</v>
+      </c>
+      <c r="H20" s="1">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1">
+        <v>3</v>
+      </c>
+      <c r="J20" s="1">
+        <v>4</v>
+      </c>
+      <c r="K20" s="1">
+        <v>4</v>
+      </c>
+      <c r="L20" s="1">
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1">
+        <v>4</v>
+      </c>
+      <c r="I21" s="1">
+        <v>4</v>
+      </c>
+      <c r="J21" s="1">
+        <v>3</v>
+      </c>
+      <c r="K21" s="1">
+        <v>3</v>
+      </c>
+      <c r="L21" s="1">
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="36">
+        <f>CORREL(B2:B22,$M$2:$M$22)</f>
+        <v>0.82640638638987718</v>
+      </c>
+      <c r="C24" s="36">
+        <f>CORREL(C2:C22,$M$2:$M$22)</f>
+        <v>0.64432393199547877</v>
+      </c>
+      <c r="D24" s="36">
+        <f>CORREL(D2:D22,$M$2:$M$22)</f>
+        <v>0.61131920365882231</v>
+      </c>
+      <c r="E24" s="36">
+        <f>CORREL(E2:E22,$M$2:$M$22)</f>
+        <v>0.56365155321390825</v>
+      </c>
+      <c r="F24" s="36">
+        <f>CORREL(F2:F22,$M$2:$M$22)</f>
+        <v>0.48886874712949885</v>
+      </c>
+      <c r="G24" s="36">
+        <f>CORREL(G2:G22,$M$2:$M$22)</f>
+        <v>0.65745650204816719</v>
+      </c>
+      <c r="H24" s="36">
+        <f>CORREL(H2:H22,$M$2:$M$22)</f>
+        <v>0.77375215704278422</v>
+      </c>
+      <c r="I24" s="36">
+        <f>CORREL(I2:I22,$M$2:$M$22)</f>
+        <v>0.62896130497169089</v>
+      </c>
+      <c r="J24" s="36">
+        <f>CORREL(J2:J22,$M$2:$M$22)</f>
+        <v>0.84261535469247029</v>
+      </c>
+      <c r="K24" s="36">
+        <f>CORREL(K2:K22,$M$2:$M$22)</f>
+        <v>0.52097256788936452</v>
+      </c>
+      <c r="L24" s="36">
+        <f>CORREL(L2:L22,$M$2:$M$22)</f>
+        <v>0.80163555951487064</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="C25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="D25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="E25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="F25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="G25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="H25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="I25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="J25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="K25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="L25" s="36">
+        <v>0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="32" t="str">
+        <f>IF(B24&gt;B25,"V","TV")</f>
+        <v>V</v>
+      </c>
+      <c r="C26" s="32" t="str">
+        <f t="shared" ref="C26:L26" si="1">IF(C24&gt;C25,"V","TV")</f>
+        <v>V</v>
+      </c>
+      <c r="D26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="E26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="F26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="G26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="H26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="I26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="J26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="K26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="L26" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>V</v>
+      </c>
+      <c r="M26" s="35">
+        <f>VAR(M2:M21)</f>
+        <v>13.186842105263157</v>
+      </c>
+      <c r="N26" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="B14" s="33">
-        <f>CORREL(B2:B11,$M$2:$M$11)</f>
-        <v>0.84307817092619819</v>
-      </c>
-      <c r="C14" s="33">
-        <f t="shared" ref="C14:L14" si="1">CORREL(C2:C11,$M$2:$M$11)</f>
-        <v>0.54900398532610239</v>
-      </c>
-      <c r="D14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.69587404584384605</v>
-      </c>
-      <c r="E14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.58881650032940824</v>
-      </c>
-      <c r="F14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.47877589854912145</v>
-      </c>
-      <c r="G14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.66651741404727849</v>
-      </c>
-      <c r="H14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.78262270248614596</v>
-      </c>
-      <c r="I14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.58881650032940824</v>
-      </c>
-      <c r="J14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.89943206106616769</v>
-      </c>
-      <c r="K14" s="33">
-        <f t="shared" si="1"/>
-        <v>0.89943206106616769</v>
-      </c>
-      <c r="L14" s="33">
-        <f>CORREL(L2:L11,$M$2:$M$11)</f>
-        <v>0.77578256389109457</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="C15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="D15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="E15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="F15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="G15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="H15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="I15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="J15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="K15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-      <c r="L15" s="33">
-        <v>0.63200000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="33" t="str">
-        <f>IF(B14&gt;B15,"Valid","Tidak Valid")</f>
-        <v>Valid</v>
-      </c>
-      <c r="C16" s="33" t="str">
-        <f t="shared" ref="C16:L16" si="2">IF(C14&gt;C15,"Valid","Tidak Valid")</f>
-        <v>Tidak Valid</v>
-      </c>
-      <c r="D16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Valid</v>
-      </c>
-      <c r="E16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Tidak Valid</v>
-      </c>
-      <c r="F16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Tidak Valid</v>
-      </c>
-      <c r="G16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Valid</v>
-      </c>
-      <c r="H16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Valid</v>
-      </c>
-      <c r="I16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Tidak Valid</v>
-      </c>
-      <c r="J16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Valid</v>
-      </c>
-      <c r="K16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Valid</v>
-      </c>
-      <c r="L16" s="33" t="str">
-        <f t="shared" si="2"/>
-        <v>Valid</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
+      <c r="B27" s="32">
+        <f>VAR(B2:B22)</f>
+        <v>0.16842105263157836</v>
+      </c>
+      <c r="C27" s="32">
+        <f>VAR(C2:C22)</f>
+        <v>0.19736842105263158</v>
+      </c>
+      <c r="D27" s="32">
+        <f>VAR(D2:D22)</f>
+        <v>0.25263157894736904</v>
+      </c>
+      <c r="E27" s="32">
+        <f>VAR(E2:E22)</f>
+        <v>0.26052631578947311</v>
+      </c>
+      <c r="F27" s="32">
+        <f>VAR(F2:F22)</f>
+        <v>0.47105263157894678</v>
+      </c>
+      <c r="G27" s="32">
+        <f>VAR(G2:G22)</f>
+        <v>0.25263157894736904</v>
+      </c>
+      <c r="H27" s="32">
+        <f>VAR(H2:H22)</f>
+        <v>0.22105263157894678</v>
+      </c>
+      <c r="I27" s="32">
+        <f>VAR(I2:I22)</f>
+        <v>0.26052631578947311</v>
+      </c>
+      <c r="J27" s="32">
+        <f>VAR(J2:J22)</f>
+        <v>0.23947368421052692</v>
+      </c>
+      <c r="K27" s="32">
+        <f>VAR(K2:K22)</f>
+        <v>0.22105263157894678</v>
+      </c>
+      <c r="L27" s="32">
+        <f>VAR(L2:L22)</f>
+        <v>0.25263157894736904</v>
+      </c>
+      <c r="M27" s="35">
+        <f>SUM(B27:L27)</f>
+        <v>2.7973684210526302</v>
+      </c>
+      <c r="N27" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="E31" s="37">
+        <f>11/10*(1-M27/M26)</f>
+        <v>0.8666533626022751</v>
+      </c>
+      <c r="F31" s="14" t="str">
+        <f>IF(AND(E31&gt;0.8,E31&lt;=1), "Reliabilias Sangat Tinggi", IF(AND(E31&gt;0.6,E31&lt;=0.8),"Relibilitas Tinggi",IF(AND(E31&gt;0.4,E31&lt;=0.6),"Relibilitas Sedang",IF(AND(E31&gt;0.2,E31&lt;=0.4),"Relibilitas Rendah",IF(AND(E31&gt;0,E31&lt;=0.2),"Tidak Reliabel","")))))</f>
+        <v>Reliabilias Sangat Tinggi</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>